<commit_message>
Fixed IPA Container test cases due to default private container exists
</commit_message>
<xml_diff>
--- a/src/test/test-data/IPAContainerTestData.xlsx
+++ b/src/test/test-data/IPAContainerTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UC196992\Git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
@@ -61,15 +66,9 @@
     <t>POST</t>
   </si>
   <si>
-    <t>X-1P-User=(SYS_USER1)||Content-Type=application/json</t>
-  </si>
-  <si>
     <t>PUT</t>
   </si>
   <si>
-    <t>X-1P-User=(SYS_USER1)</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
@@ -82,9 +81,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>status=200||public_count=0||private_count=0||total_count=0</t>
-  </si>
-  <si>
     <t>{ "ispublic": true }</t>
   </si>
   <si>
@@ -103,9 +99,6 @@
     <t>X-1P-User=(SYS_USER2)</t>
   </si>
   <si>
-    <t>status=200||public_count=1||private_count=1||total_count=2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that saved work counts are shown as zero when user doesn't have any saved works using container API. </t>
   </si>
   <si>
@@ -136,9 +129,6 @@
     <t>{"name":"First IPA Container by Project Neon1","type":"ipa_ss","ispublic":false, "desc": "First SSE - IPA Container created by postman"}</t>
   </si>
   <si>
-    <t>status=200||type=ipa_ss||name=First IPA Container by Project Neon1||desc=First SSE - IPA Container created by postman||userid=(SYS_USER1)||ispublic=false||isOwner=false</t>
-  </si>
-  <si>
     <t>Verify that user is able to create multiple containers for IPA saved works using container API</t>
   </si>
   <si>
@@ -148,21 +138,12 @@
     <t>{"name":"Second IPA Container by Project Neon1","type":"ipa_ss","ispublic":false, "desc": "Second SSE - IPA Container created by postman"}</t>
   </si>
   <si>
-    <t>status=200||type=ipa_ss||name=Second IPA Container by Project Neon1||desc=Second SSE - IPA Container created by postman||userid=(SYS_USER1)||ispublic=false||isOwner=false</t>
-  </si>
-  <si>
     <t>{ "name": "IPA Container name updated from API" }</t>
   </si>
   <si>
-    <t>status=200||type=ipa_ss||name=IPA Container name updated from API||desc=First SSE - IPA Container created by postman||userid=(SYS_USER1)||ispublic=false||isOwner=false</t>
-  </si>
-  <si>
     <t>{ "desc": "IPA container 1 updated description from API" }</t>
   </si>
   <si>
-    <t>status=200||type=ipa_ss||name=IPA Container name updated from API||desc=IPA container 1 updated description from API||userid=(SYS_USER1)||ispublic=false||isOwner=false</t>
-  </si>
-  <si>
     <t>Verify that user is able to update IPA container status using container API</t>
   </si>
   <si>
@@ -175,9 +156,6 @@
     <t>?itemType=ipa_sse&amp;sortoption=latestupdated</t>
   </si>
   <si>
-    <t>status=200||type=ipa_ss||name=Second IPA Container by Project Neon1||desc=Second SSE - IPA Container created by postman||userid=(SYS_USER1)||ispublic=true||isOwner=false</t>
-  </si>
-  <si>
     <t>Verify that user is able to add saved work for technology type to a particular IPA container using container API</t>
   </si>
   <si>
@@ -262,9 +240,6 @@
     <t>/container/(OPQA-4567_id)</t>
   </si>
   <si>
-    <t>status=200||public_count=1||private_count=1||total_count=2||private[0].id=(OPQA-4566_id)||private[0].contents.ipa_sse=4||private[0].contents.total=4||public[0].id=(OPQA-4567_id)||public[0].contents.ipa_sse=0||public[0].contents.total=0</t>
-  </si>
-  <si>
     <t>OPQA-4568</t>
   </si>
   <si>
@@ -347,13 +322,43 @@
   </si>
   <si>
     <t>OPQA-4635</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER3)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>status=200||type=ipa_ss||name=First IPA Container by Project Neon1||desc=First SSE - IPA Container created by postman||userid=(SYS_USER2)||ispublic=false||isOwner=false</t>
+  </si>
+  <si>
+    <t>status=200||type=ipa_ss||name=Second IPA Container by Project Neon1||desc=Second SSE - IPA Container created by postman||userid=(SYS_USER2)||ispublic=false||isOwner=false</t>
+  </si>
+  <si>
+    <t>status=200||type=ipa_ss||name=IPA Container name updated from API||desc=First SSE - IPA Container created by postman||userid=(SYS_USER2)||ispublic=false||isOwner=false</t>
+  </si>
+  <si>
+    <t>status=200||type=ipa_ss||name=IPA Container name updated from API||desc=IPA container 1 updated description from API||userid=(SYS_USER2)||ispublic=false||isOwner=false</t>
+  </si>
+  <si>
+    <t>status=200||type=ipa_ss||name=Second IPA Container by Project Neon1||desc=Second SSE - IPA Container created by postman||userid=(SYS_USER2)||ispublic=true||isOwner=false</t>
+  </si>
+  <si>
+    <t>status=200||public_count=0||private_count=1||total_count=1</t>
+  </si>
+  <si>
+    <t>status=200||public_count=1||private_count=2||total_count=3</t>
+  </si>
+  <si>
+    <t>status=200||public_count=1||private_count=2||total_count=3||private[0].id=(OPQA-4566_id)||private[0].contents.ipa_sse=4||private[0].contents.total=4||public[0].id=(OPQA-4567_id)||public[0].contents.ipa_sse=0||public[0].contents.total=0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,6 +474,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -515,7 +528,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -547,9 +560,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -581,6 +595,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -756,14 +771,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L2:L26"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="44.85546875" style="3" customWidth="1" collapsed="1"/>
@@ -779,7 +794,7 @@
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
@@ -817,251 +832,251 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="47.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2"/>
       <c r="J2" s="2" t="s">
-        <v>22</v>
+        <v>108</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I3"/>
       <c r="J3" s="2" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L3"/>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G4"/>
       <c r="H4" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I4"/>
       <c r="J4" s="2" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G5"/>
       <c r="H5" s="11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G6"/>
       <c r="H6" s="11" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G7"/>
       <c r="H7" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="60">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="G8"/>
       <c r="H8" s="11" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="30">
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H9"/>
       <c r="I9" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>13</v>
@@ -1069,538 +1084,538 @@
       <c r="K9" s="2"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="30">
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
       <c r="I10" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="K10"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G11"/>
       <c r="H11" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" ht="47.25">
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="120">
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" s="1" customFormat="1" ht="135">
+    <row r="17" spans="1:12" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H17" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="J17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" s="1" customFormat="1" ht="135">
+    <row r="18" spans="1:12" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G18"/>
       <c r="H18" s="11" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" s="1" customFormat="1" ht="60">
+    <row r="19" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G19"/>
       <c r="H19" s="11" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" s="1" customFormat="1" ht="135">
+    <row r="20" spans="1:12" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" s="1" customFormat="1" ht="60">
+    <row r="21" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12" s="1" customFormat="1" ht="45">
+    <row r="22" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12" ht="30">
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="45">
+    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:12" ht="30">
+    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="45">
+    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>